<commit_message>
Adding energy and emissions datasets and calculations
</commit_message>
<xml_diff>
--- a/Data/3_MC_Elements_Materials_ExistingStock_V2.0.xlsx
+++ b/Data/3_MC_Elements_Materials_ExistingStock_V2.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13692" windowHeight="5376" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13692" windowHeight="5376"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>RECC_Classifications_Master_V1.0</t>
-  </si>
-  <si>
     <t>3_MC_Elements_Materials_ExistingStock</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>cement</t>
+  </si>
+  <si>
+    <t>RECC_Classifications_Master_V2.0</t>
   </si>
 </sst>
 </file>
@@ -464,9 +464,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent 4" xfId="2"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -770,11 +770,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.109375" customWidth="1"/>
@@ -818,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
@@ -833,7 +833,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
@@ -890,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
@@ -905,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
@@ -920,7 +920,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
@@ -980,7 +980,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
@@ -995,7 +995,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
@@ -1094,16 +1094,16 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>24</v>
@@ -1117,16 +1117,16 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>24</v>
@@ -1292,11 +1292,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3031"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
@@ -1309,10 +1309,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>53</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1344,17 +1344,17 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1366,17 +1366,17 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1388,17 +1388,17 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1410,17 +1410,17 @@
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1432,17 +1432,17 @@
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1454,17 +1454,17 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1476,17 +1476,17 @@
         <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1498,17 +1498,17 @@
         <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1520,17 +1520,17 @@
         <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1542,17 +1542,17 @@
         <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1564,16 +1564,16 @@
         <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1585,16 +1585,16 @@
         <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1606,16 +1606,16 @@
         <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1627,15 +1627,15 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1647,15 +1647,15 @@
         <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1667,7 +1667,7 @@
         <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -1676,10 +1676,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1691,7 +1691,7 @@
         <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -1700,10 +1700,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19">
         <v>0.99</v>
@@ -1715,7 +1715,7 @@
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
@@ -1724,10 +1724,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20">
         <v>0.99</v>
@@ -1739,7 +1739,7 @@
         <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
@@ -1772,10 +1772,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>26</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
@@ -1796,10 +1796,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1811,7 +1811,7 @@
         <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -1820,10 +1820,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1835,7 +1835,7 @@
         <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
@@ -1844,10 +1844,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1859,7 +1859,7 @@
         <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -1868,10 +1868,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1883,7 +1883,7 @@
         <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1907,7 +1907,7 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1931,7 +1931,7 @@
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>0.01</v>
@@ -1955,15 +1955,15 @@
         <v>26</v>
       </c>
       <c r="F29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30">
         <v>0.08</v>
@@ -1975,15 +1975,15 @@
         <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1995,16 +1995,16 @@
         <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2016,16 +2016,16 @@
         <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2037,17 +2037,17 @@
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H33" s="9"/>
       <c r="K33" s="9"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2059,7 +2059,7 @@
         <v>26</v>
       </c>
       <c r="F34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H34" s="9"/>
       <c r="K34" s="9"/>
@@ -2067,10 +2067,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2082,7 +2082,7 @@
         <v>26</v>
       </c>
       <c r="F35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H35" s="9"/>
       <c r="K35" s="9"/>
@@ -2090,10 +2090,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2105,7 +2105,7 @@
         <v>26</v>
       </c>
       <c r="F36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H36" s="9"/>
       <c r="K36" s="9"/>
@@ -2113,10 +2113,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2128,7 +2128,7 @@
         <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H37" s="9"/>
       <c r="K37" s="9"/>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2151,7 +2151,7 @@
         <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -2160,10 +2160,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2175,7 +2175,7 @@
         <v>26</v>
       </c>
       <c r="F39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -2184,10 +2184,10 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2199,7 +2199,7 @@
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -2208,10 +2208,10 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41">
         <v>0.999</v>
@@ -2223,7 +2223,7 @@
         <v>26</v>
       </c>
       <c r="F41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -2232,10 +2232,10 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42">
         <v>0.9899</v>
@@ -2247,7 +2247,7 @@
         <v>26</v>
       </c>
       <c r="F42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -2256,10 +2256,10 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43">
         <v>0.86</v>
@@ -2271,7 +2271,7 @@
         <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44">
         <v>0.999</v>
@@ -2295,7 +2295,7 @@
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -2304,10 +2304,10 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2319,7 +2319,7 @@
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2343,7 +2343,7 @@
         <v>26</v>
       </c>
       <c r="F46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
@@ -2352,10 +2352,10 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2367,7 +2367,7 @@
         <v>26</v>
       </c>
       <c r="F47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -2376,10 +2376,10 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2391,7 +2391,7 @@
         <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2415,7 +2415,7 @@
         <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -2424,10 +2424,10 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2439,7 +2439,7 @@
         <v>26</v>
       </c>
       <c r="F50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
@@ -2448,10 +2448,10 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>26</v>
       </c>
       <c r="F51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -2471,10 +2471,10 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2486,7 +2486,7 @@
         <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2509,7 +2509,7 @@
         <v>26</v>
       </c>
       <c r="F53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
@@ -2518,10 +2518,10 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2533,7 +2533,7 @@
         <v>26</v>
       </c>
       <c r="F54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
@@ -2542,10 +2542,10 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2557,7 +2557,7 @@
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2581,7 +2581,7 @@
         <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
@@ -2590,10 +2590,10 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2605,7 +2605,7 @@
         <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
@@ -2614,10 +2614,10 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58">
         <v>0.01</v>
@@ -2629,7 +2629,7 @@
         <v>26</v>
       </c>
       <c r="F58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -2638,10 +2638,10 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59">
         <v>0.01</v>
@@ -2653,7 +2653,7 @@
         <v>26</v>
       </c>
       <c r="F59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
@@ -2662,10 +2662,10 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2677,7 +2677,7 @@
         <v>26</v>
       </c>
       <c r="F60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
@@ -2686,10 +2686,10 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2701,7 +2701,7 @@
         <v>26</v>
       </c>
       <c r="F61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
@@ -2710,10 +2710,10 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -2725,7 +2725,7 @@
         <v>26</v>
       </c>
       <c r="F62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
@@ -2734,10 +2734,10 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2749,7 +2749,7 @@
         <v>26</v>
       </c>
       <c r="F63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
@@ -2758,10 +2758,10 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2773,7 +2773,7 @@
         <v>26</v>
       </c>
       <c r="F64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
@@ -2782,10 +2782,10 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2797,7 +2797,7 @@
         <v>26</v>
       </c>
       <c r="F65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2821,16 +2821,16 @@
         <v>26</v>
       </c>
       <c r="F66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H66" s="9"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67">
         <v>1E-3</v>
@@ -2842,16 +2842,16 @@
         <v>26</v>
       </c>
       <c r="F67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H67" s="9"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C68">
         <v>1E-4</v>
@@ -2863,16 +2863,16 @@
         <v>26</v>
       </c>
       <c r="F68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H68" s="9"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C69">
         <v>0.06</v>
@@ -2884,16 +2884,16 @@
         <v>26</v>
       </c>
       <c r="F69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H69" s="9"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70">
         <v>1E-3</v>
@@ -2905,16 +2905,16 @@
         <v>26</v>
       </c>
       <c r="F70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H70" s="9"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2926,16 +2926,16 @@
         <v>26</v>
       </c>
       <c r="F71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H71" s="9"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2947,16 +2947,16 @@
         <v>26</v>
       </c>
       <c r="F72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H72" s="9"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2968,15 +2968,15 @@
         <v>26</v>
       </c>
       <c r="F73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2988,15 +2988,15 @@
         <v>26</v>
       </c>
       <c r="F74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -3008,15 +3008,15 @@
         <v>26</v>
       </c>
       <c r="F75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -3028,15 +3028,15 @@
         <v>26</v>
       </c>
       <c r="F76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -3048,15 +3048,15 @@
         <v>26</v>
       </c>
       <c r="F77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -3068,15 +3068,15 @@
         <v>26</v>
       </c>
       <c r="F78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -3088,15 +3088,15 @@
         <v>26</v>
       </c>
       <c r="F79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3108,15 +3108,15 @@
         <v>26</v>
       </c>
       <c r="F80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3128,7 +3128,7 @@
         <v>26</v>
       </c>
       <c r="F81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -20875,7 +20875,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" style="22"/>
     <col min="2" max="2" width="43" style="22" bestFit="1" customWidth="1"/>

</xml_diff>